<commit_message>
Updated the first pipe, and the last pipe with graphics
</commit_message>
<xml_diff>
--- a/Maps/Mønster til TD spill.xlsx
+++ b/Maps/Mønster til TD spill.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10720" yWindow="4680" windowWidth="47800" windowHeight="25940" tabRatio="500"/>
+    <workbookView xWindow="26560" yWindow="620" windowWidth="33600" windowHeight="33220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Map 1" sheetId="2" r:id="rId1"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="AH20" sqref="AH20:AH52"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <selection activeCell="AW32" sqref="AW32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3480,7 +3480,7 @@
         <v>21</v>
       </c>
       <c r="AV41" s="20">
-        <v>270</v>
+        <v>360</v>
       </c>
       <c r="AW41" s="20">
         <v>360</v>
@@ -3549,7 +3549,7 @@
         <v>22</v>
       </c>
       <c r="AV42" s="20">
-        <v>360</v>
+        <v>450</v>
       </c>
       <c r="AW42" s="20">
         <v>360</v>
@@ -3619,7 +3619,7 @@
         <v>23</v>
       </c>
       <c r="AV43" s="20">
-        <v>450</v>
+        <v>540</v>
       </c>
       <c r="AW43" s="20">
         <v>360</v>
@@ -3670,7 +3670,7 @@
         <v>90</v>
       </c>
       <c r="AH44" s="20">
-        <f t="shared" ref="AH44:AH47" si="3">AH43-90</f>
+        <f t="shared" ref="AH44" si="3">AH43-90</f>
         <v>450</v>
       </c>
       <c r="AI44" s="3"/>
@@ -3758,7 +3758,7 @@
         <v>25</v>
       </c>
       <c r="AV45" s="20">
-        <v>540</v>
+        <v>630</v>
       </c>
       <c r="AW45" s="20">
         <v>270</v>
@@ -3965,7 +3965,7 @@
         <v>28</v>
       </c>
       <c r="AV48" s="20">
-        <v>630</v>
+        <v>540</v>
       </c>
       <c r="AW48" s="20">
         <v>90</v>
@@ -4029,7 +4029,7 @@
         <v>29</v>
       </c>
       <c r="AV49" s="20">
-        <v>540</v>
+        <v>450</v>
       </c>
       <c r="AW49" s="20">
         <v>90</v>
@@ -4067,7 +4067,7 @@
         <v>30</v>
       </c>
       <c r="AV50" s="20">
-        <v>450</v>
+        <v>360</v>
       </c>
       <c r="AW50">
         <v>90</v>

</xml_diff>